<commit_message>
Update after IROS paper finished
</commit_message>
<xml_diff>
--- a/multiuser_legible_movement/data/eval/simulation_results_b.xlsx
+++ b/multiuser_legible_movement/data/eval/simulation_results_b.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\My_documents\Instituto.Superior.Tecnico\PhD\movement_communication\multiuser_legible_movement\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\My_documents\Instituto.Superior.Tecnico\PhD\movement_communication\multiuser_legible_movement\data\eval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A41D66-4CD4-4656-83E8-75725BCEB7BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5FAEDE-1799-4440-BDF2-5CCB42338884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="6">
   <si>
     <t>Configuration</t>
   </si>
@@ -42,148 +42,7 @@
     <t>User 3</t>
   </si>
   <si>
-    <t>User 1: 0.46456
-User 2: 0.42451
-User 3: 0.33135
-Average: 0.40680</t>
-  </si>
-  <si>
-    <t>User 1: 0.47774
-User 2: 0.00000
-User 3: 0.35296
-Average: 0.27690</t>
-  </si>
-  <si>
-    <t>User 1: 0.46937
-User 2: 0.38708
-User 3: 0.32055
-Average: 0.39233</t>
-  </si>
-  <si>
-    <t>User 1: 0.48147
-User 2: 0.00000
-User 3: 0.45670
-Average: 0.31273</t>
-  </si>
-  <si>
-    <t>User 1: 0.41660
-User 2: 0.34126
-User 3: 0.32737
-Average: 0.36174</t>
-  </si>
-  <si>
-    <t>User 1: 0.44777
-User 2: 0.41729
-User 3: 0.34507
-Average: 0.40338</t>
-  </si>
-  <si>
-    <t>User 1: 0.24031
-User 2: 0.33596
-User 3: 0.32489
-Average: 0.30039</t>
-  </si>
-  <si>
-    <t>User 1: 0.42351
-User 2: 0.16401
-User 3: 0.45581
-Average: 0.34778</t>
-  </si>
-  <si>
-    <t>User 1: 0.34727
-User 2: 0.33540
-User 3: 0.34022
-Average: 0.34096</t>
-  </si>
-  <si>
-    <t>User 1: 0.35995
-User 2: 0.34433
-User 3: 0.33998
-Average: 0.34809</t>
-  </si>
-  <si>
-    <t>User 1: 0.34047
-User 2: 0.33514
-User 3: 0.33537
-Average: 0.33699</t>
-  </si>
-  <si>
-    <t>User 1: 0.37273
-User 2: 0.32891
-User 3: 0.41208
-Average: 0.37124</t>
-  </si>
-  <si>
-    <t>User 1: 0.45014
-User 2: 0.41955
-User 3: 0.39269
-Average: 0.42079</t>
-  </si>
-  <si>
-    <t>User 1: 0.47025
-User 2: 0.43405
-User 3: 0.39587
-Average: 0.43339</t>
-  </si>
-  <si>
-    <t>User 1: 0.42070
-User 2: 0.41791
-User 3: 0.40092
-Average: 0.41318</t>
-  </si>
-  <si>
-    <t>User 1: 0.33493
-User 2: 0.38051
-User 3: 0.38128
-Average: 0.36557</t>
-  </si>
-  <si>
-    <t>User 1: 0.33413
-User 2: 0.33548
-User 3: 0.34925
-Average: 0.33962</t>
-  </si>
-  <si>
-    <t>User 1: 0.33951
-User 2: 0.33005
-User 3: 0.33509
-Average: 0.33488</t>
-  </si>
-  <si>
-    <t>User 1: 0.33506
-User 2: 0.34622
-User 3: 0.36168
-Average: 0.34765</t>
-  </si>
-  <si>
-    <t>User 1: 0.33439
-User 2: 0.33566
-User 3: 0.35187
-Average: 0.34064</t>
-  </si>
-  <si>
-    <t>User 1: 0.42758
-User 2: 0.36915
-User 3: 0.35042
-Average: 0.38238</t>
-  </si>
-  <si>
-    <t>User 1: 0.41980
-User 2: 0.39534
-User 3: 0.35807
-Average: 0.39107</t>
-  </si>
-  <si>
-    <t>User 1: 0.40240
-User 2: 0.41546
-User 3: 0.35848
-Average: 0.39211</t>
-  </si>
-  <si>
-    <t>User 1: 0.22584
-User 2: 0.36997
-User 3: 0.36311
-Average: 0.31964</t>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -206,7 +65,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -229,17 +88,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,141 +472,470 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C18" sqref="C18:F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875"/>
-    <col min="2" max="5" width="15.7265625" customWidth="1"/>
-    <col min="6" max="1025" width="11.54296875"/>
+    <col min="1" max="16384" width="10.6328125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="50" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.56877999999999995</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.56794999999999995</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.56315000000000004</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.56315000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.47615000000000002</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.47969000000000001</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.48196</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.46095000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.47615000000000002</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.47969000000000001</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.46095000000000003</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.48196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C5" s="5">
+        <v>0.50702999999999998</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.50910999999999995</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.50202000000000002</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.50202000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.36148000000000002</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.36149999999999999</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.36147000000000001</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.36147000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.38534000000000002</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.38529999999999998</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.38535000000000003</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.38532</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.38534000000000002</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.38529999999999998</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.38532</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.38535000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.37737999999999999</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.37736999999999998</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.37737999999999999</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.37737999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.34655000000000002</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.34656999999999999</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.34655000000000002</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.34655000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.35693000000000003</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.35665000000000002</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.35693999999999998</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.35692000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.35693000000000003</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.35665000000000002</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.35692000000000002</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.35693999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.35347000000000001</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.35328999999999999</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.35347000000000001</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.35347000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.57381000000000004</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.87294000000000005</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.55506999999999995</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.31075999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.81179999999999997</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.93650999999999995</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.9365</v>
+      </c>
+      <c r="F15" s="4">
+        <v>3.3099999999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.33217000000000002</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>3.175E-2</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.83370999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.57259000000000004</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.60314999999999996</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.50777000000000005</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.39251999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="B18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="8">
+        <v>0.84706000000000004</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0.93647999999999998</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0.51439999999999997</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.51439999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.29202</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.39080999999999999</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.38790000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.29202</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.38790000000000002</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.39080999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.47704000000000002</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.31215999999999999</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.43103000000000002</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.43103000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="50" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="B22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="50" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="50" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="50" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="50" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>